<commit_message>
ADD 18 and 13 solutions
</commit_message>
<xml_diff>
--- a/Others_Solutions/Ст. Инф. 02.02.2021/1921/1921.xlsx
+++ b/Others_Solutions/Ст. Инф. 02.02.2021/1921/1921.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hem12\Documents\Документы Миша\Школьные предметы\ЕГЭ информатика\Solutions\PrepareForEGE_MishaPolykovsky\Others_Solutions\Ст. Инф. 02.02.2021\1921\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CAA1F1-4E08-4FC1-B5D4-E8716F98F113}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFED79C-68FE-4B27-B4B9-B81D207888C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,8 +51,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,6 +102,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -119,11 +132,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1"/>
@@ -132,8 +146,10 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Акцент5" xfId="2" builtinId="45"/>
     <cellStyle name="Вывод" xfId="1" builtinId="21"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -197,6 +213,59 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Прямая со стрелкой 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{113E6904-155A-437B-A894-9523DC99622F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5800725" y="1219200"/>
+          <a:ext cx="9525" cy="3857625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent5"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -474,7 +543,7 @@
   <dimension ref="E6:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AA12" sqref="Z12:AA12"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +603,7 @@
         <v>34</v>
       </c>
       <c r="Y6">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="5:25" x14ac:dyDescent="0.25">
@@ -545,7 +614,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="6"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="8"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>

</xml_diff>